<commit_message>
fix: 修复table-utils-> isEmptyCell 判断bug,增加测试 affects: @ailhc/excel2all
</commit_message>
<xml_diff>
--- a/tool-packages/excel2all/__test__/test-excel-files/MergeTableFolder1/MergeTableSetting.xlsx
+++ b/tool-packages/excel2all/__test__/test-excel-files/MergeTableFolder1/MergeTableSetting.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540"/>
+    <workbookView windowWidth="28125" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="测试数据" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <author>AILHC</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="59">
   <si>
     <t>MergeTableSetting</t>
   </si>
@@ -60,6 +60,9 @@
     <t>数字</t>
   </si>
   <si>
+    <t>布尔值</t>
+  </si>
+  <si>
     <t>数字数组</t>
   </si>
   <si>
@@ -93,6 +96,9 @@
     <t>int</t>
   </si>
   <si>
+    <t>boolean</t>
+  </si>
+  <si>
     <t>[int]</t>
   </si>
   <si>
@@ -129,6 +135,9 @@
     <t>field_int</t>
   </si>
   <si>
+    <t>field_bool</t>
+  </si>
+  <si>
     <t>field_int_array</t>
   </si>
   <si>
@@ -214,6 +223,9 @@
   </si>
   <si>
     <t>同名表合并测试，第二张表</t>
+  </si>
+  <si>
+    <t>SERVER 我这边用于服务端字段 可以是任意类型的标志，可自定义解析</t>
   </si>
 </sst>
 </file>
@@ -221,9 +233,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -242,8 +254,107 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -258,47 +369,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -310,83 +384,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -412,43 +424,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,133 +562,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,25 +616,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -642,6 +636,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -653,21 +662,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -689,6 +683,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -697,153 +700,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1191,30 +1203,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AQ1171"/>
+  <dimension ref="A1:AR1171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="19.375" customWidth="1"/>
     <col min="2" max="2" width="27.125" customWidth="1"/>
-    <col min="3" max="3" width="10.375" customWidth="1"/>
-    <col min="4" max="4" width="17.125" customWidth="1"/>
-    <col min="5" max="5" width="13.75" customWidth="1"/>
-    <col min="6" max="6" width="30.375" customWidth="1"/>
-    <col min="7" max="7" width="28.25" customWidth="1"/>
-    <col min="8" max="8" width="19.375" customWidth="1"/>
-    <col min="9" max="9" width="22.625" customWidth="1"/>
-    <col min="10" max="10" width="26" customWidth="1"/>
-    <col min="11" max="11" width="30.375" customWidth="1"/>
-    <col min="12" max="15" width="14.875" customWidth="1"/>
-    <col min="16" max="17" width="16.125" customWidth="1"/>
+    <col min="3" max="4" width="10.375" customWidth="1"/>
+    <col min="5" max="5" width="17.125" customWidth="1"/>
+    <col min="6" max="6" width="13.75" customWidth="1"/>
+    <col min="7" max="7" width="30.375" customWidth="1"/>
+    <col min="8" max="8" width="28.25" customWidth="1"/>
+    <col min="9" max="9" width="19.375" customWidth="1"/>
+    <col min="10" max="10" width="22.625" customWidth="1"/>
+    <col min="11" max="11" width="26" customWidth="1"/>
+    <col min="12" max="12" width="30.375" customWidth="1"/>
+    <col min="13" max="16" width="14.875" customWidth="1"/>
+    <col min="17" max="18" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:43">
+    <row r="1" s="1" customFormat="1" spans="1:44">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1251,48 +1263,53 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="AQ1" s="4"/>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2"/>
+      <c r="AR1" s="4"/>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="2"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -1300,61 +1317,65 @@
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="V2" s="4"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="4"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1363,267 +1384,287 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>37</v>
+      <c r="D5" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="2">
+        <v>5</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="2">
-        <v>5</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K5" t="s">
-        <v>39</v>
-      </c>
       <c r="L5" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13">
+        <v>42</v>
+      </c>
+      <c r="M5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="2"/>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C6" s="2">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>37</v>
+      <c r="D6" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
         <v>42</v>
       </c>
-      <c r="F6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="2">
+        <v>8</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="2">
-        <v>8</v>
-      </c>
-      <c r="I6" s="2" t="s">
+      <c r="L6" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="M6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2">
         <v>60000</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>44</v>
+      <c r="D7" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
+        <v>47</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="2">
+        <v>60000</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="2">
-        <v>60000</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="F8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K8" t="s">
-        <v>47</v>
-      </c>
       <c r="L8" t="s">
-        <v>40</v>
-      </c>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13">
+        <v>50</v>
+      </c>
+      <c r="M8" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="2"/>
       <c r="B9" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2">
         <v>6</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>49</v>
+      <c r="D9" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" t="s">
-        <v>47</v>
+        <v>52</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="2">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="2">
         <v>6</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="J9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="K9" t="s">
-        <v>47</v>
+        <v>41</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="L9" t="s">
-        <v>40</v>
-      </c>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13">
+        <v>50</v>
+      </c>
+      <c r="M9" t="s">
+        <v>43</v>
+      </c>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="2"/>
       <c r="B10" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C10" s="2">
         <v>0.5</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>37</v>
+      <c r="D10" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" t="s">
-        <v>47</v>
+        <v>40</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="G10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" t="s">
-        <v>47</v>
-      </c>
       <c r="L10" t="s">
-        <v>40</v>
-      </c>
-      <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="1:13">
+        <v>50</v>
+      </c>
+      <c r="M10" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C11" s="2">
         <v>300</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" t="s">
-        <v>47</v>
+        <v>56</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="2">
+        <v>50</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="2">
         <v>300</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="J11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K11" t="s">
-        <v>47</v>
+        <v>41</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="L11" t="s">
-        <v>40</v>
-      </c>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:13">
+        <v>50</v>
+      </c>
+      <c r="M11" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1637,8 +1678,9 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1652,8 +1694,9 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1667,8 +1710,9 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1682,8 +1726,9 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1697,8 +1742,9 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1712,8 +1758,9 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1727,8 +1774,9 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1742,8 +1790,9 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1757,8 +1806,9 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1772,8 +1822,9 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1787,8 +1838,9 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1802,8 +1854,9 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1817,8 +1870,9 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1832,8 +1886,9 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="N25" s="2"/>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1847,11 +1902,12 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1864,8 +1920,9 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1879,71 +1936,77 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
-    </row>
-    <row r="29" spans="6:7">
-      <c r="F29" s="4"/>
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="7:8">
       <c r="G29" s="4"/>
-    </row>
-    <row r="32" spans="6:7">
-      <c r="F32" s="4"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="7:8">
       <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="6:7">
-      <c r="F33" s="4"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="7:8">
       <c r="G33" s="4"/>
-    </row>
-    <row r="36" spans="6:7">
-      <c r="F36" s="4"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="36" spans="7:8">
       <c r="G36" s="4"/>
-    </row>
-    <row r="37" spans="6:7">
-      <c r="F37" s="4"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="7:8">
       <c r="G37" s="4"/>
-    </row>
-    <row r="40" spans="6:7">
-      <c r="F40" s="4"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="40" spans="7:8">
       <c r="G40" s="4"/>
-    </row>
-    <row r="41" spans="6:7">
-      <c r="F41" s="4"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="7:8">
       <c r="G41" s="4"/>
-    </row>
-    <row r="42" spans="6:7">
-      <c r="F42" s="4"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="7:8">
       <c r="G42" s="4"/>
-    </row>
-    <row r="43" spans="6:7">
-      <c r="F43" s="4"/>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="7:8">
       <c r="G43" s="4"/>
-    </row>
-    <row r="44" spans="6:7">
-      <c r="F44" s="4"/>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="7:8">
       <c r="G44" s="4"/>
-    </row>
-    <row r="45" spans="6:7">
-      <c r="F45" s="4"/>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="7:8">
       <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
     </row>
     <row r="1171" spans="1:1">
       <c r="A1171" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F5 F6:F11">
+  <conditionalFormatting sqref="G5:G11">
     <cfRule type="cellIs" dxfId="0" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5 G6:G11">
+  <conditionalFormatting sqref="H5:H11">
     <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K5 K6:K11">
+  <conditionalFormatting sqref="L5:L11">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L5 L6:L11">
+  <conditionalFormatting sqref="M5:M11">
     <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>

</xml_diff>